<commit_message>
Update PNM Schedule 1 Censored.xlsx
</commit_message>
<xml_diff>
--- a/PNM Schedule 1 Censored.xlsx
+++ b/PNM Schedule 1 Censored.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chaos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\Recruitment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E592F7F-4773-4013-A130-B94E681C9D74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761AF3A7-E5FC-4B01-A102-12EF94F08D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2730" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DailySchedulePnmSchedule" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="19">
   <si>
     <t>A</t>
   </si>
@@ -59,6 +59,27 @@
   </si>
   <si>
     <t>Slot 4</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Group 5</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>Group 3</t>
+  </si>
+  <si>
+    <t>Group 6</t>
+  </si>
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Group 4</t>
   </si>
 </sst>
 </file>
@@ -416,18 +437,21 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
@@ -445,6 +469,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -462,6 +489,9 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -476,6 +506,9 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -493,6 +526,9 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -509,6 +545,9 @@
     <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -527,6 +566,9 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -544,6 +586,9 @@
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
@@ -561,6 +606,9 @@
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
@@ -578,6 +626,9 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
@@ -595,6 +646,9 @@
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
@@ -612,6 +666,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
@@ -623,6 +680,9 @@
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
@@ -640,6 +700,9 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
@@ -657,6 +720,9 @@
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
@@ -674,6 +740,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
@@ -691,6 +760,9 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
@@ -702,6 +774,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
@@ -719,6 +794,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
@@ -736,6 +814,9 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
       <c r="C20" t="s">
         <v>2</v>
       </c>
@@ -753,6 +834,9 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
       <c r="C21" t="s">
         <v>3</v>
       </c>
@@ -770,6 +854,9 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
       <c r="C22" t="s">
         <v>3</v>
       </c>
@@ -787,6 +874,9 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
       <c r="D23" t="s">
         <v>0</v>
       </c>
@@ -801,6 +891,9 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
       <c r="C24" t="s">
         <v>1</v>
       </c>
@@ -818,6 +911,9 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
       <c r="C25" t="s">
         <v>3</v>
       </c>
@@ -835,6 +931,9 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
@@ -852,6 +951,9 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -869,6 +971,9 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
       <c r="C28" t="s">
         <v>2</v>
       </c>
@@ -886,6 +991,9 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
       <c r="C29" t="s">
         <v>3</v>
       </c>
@@ -903,6 +1011,9 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
@@ -920,6 +1031,9 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
       <c r="C31" t="s">
         <v>3</v>
       </c>
@@ -937,6 +1051,9 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
       <c r="C32" t="s">
         <v>2</v>
       </c>
@@ -954,6 +1071,9 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
       <c r="C33" t="s">
         <v>0</v>
       </c>
@@ -971,6 +1091,9 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
@@ -988,6 +1111,9 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
       <c r="C35" t="s">
         <v>0</v>
       </c>
@@ -1005,6 +1131,9 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" t="s">
+        <v>17</v>
+      </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
@@ -1019,6 +1148,9 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
@@ -1027,6 +1159,9 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
@@ -1044,6 +1179,9 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
@@ -1061,6 +1199,9 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
@@ -1078,6 +1219,9 @@
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
@@ -1095,6 +1239,9 @@
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
       <c r="C42" t="s">
         <v>3</v>
       </c>
@@ -1112,6 +1259,9 @@
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
       <c r="C43" t="s">
         <v>2</v>
       </c>
@@ -1129,6 +1279,9 @@
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44" t="s">
+        <v>17</v>
+      </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
@@ -1140,6 +1293,9 @@
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
@@ -1157,6 +1313,9 @@
       <c r="A46">
         <v>45</v>
       </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
       <c r="C46" t="s">
         <v>5</v>
       </c>
@@ -1174,6 +1333,9 @@
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
@@ -1191,6 +1353,9 @@
       <c r="A48">
         <v>47</v>
       </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
       <c r="C48" t="s">
         <v>4</v>
       </c>
@@ -1208,6 +1373,9 @@
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
       <c r="C49" t="s">
         <v>2</v>
       </c>
@@ -1225,6 +1393,9 @@
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" t="s">
+        <v>16</v>
+      </c>
       <c r="C50" t="s">
         <v>1</v>
       </c>
@@ -1242,6 +1413,9 @@
       <c r="A51">
         <v>50</v>
       </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
@@ -1259,6 +1433,9 @@
       <c r="A52">
         <v>51</v>
       </c>
+      <c r="B52" t="s">
+        <v>17</v>
+      </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
@@ -1276,6 +1453,9 @@
       <c r="A53">
         <v>52</v>
       </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
       <c r="C53" t="s">
         <v>6</v>
       </c>
@@ -1293,6 +1473,9 @@
       <c r="A54">
         <v>53</v>
       </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
       <c r="C54" t="s">
         <v>4</v>
       </c>
@@ -1310,6 +1493,9 @@
       <c r="A55">
         <v>54</v>
       </c>
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
       <c r="C55" t="s">
         <v>3</v>
       </c>
@@ -1327,6 +1513,9 @@
       <c r="A56">
         <v>55</v>
       </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
@@ -1341,6 +1530,9 @@
       <c r="A57">
         <v>56</v>
       </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
       <c r="C57" t="s">
         <v>5</v>
       </c>
@@ -1355,6 +1547,9 @@
       <c r="A58">
         <v>57</v>
       </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
       <c r="C58" t="s">
         <v>5</v>
       </c>
@@ -1372,6 +1567,9 @@
       <c r="A59">
         <v>58</v>
       </c>
+      <c r="B59" t="s">
+        <v>14</v>
+      </c>
       <c r="D59" t="s">
         <v>5</v>
       </c>
@@ -1386,6 +1584,9 @@
       <c r="A60">
         <v>59</v>
       </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
       <c r="C60" t="s">
         <v>4</v>
       </c>
@@ -1403,6 +1604,9 @@
       <c r="A61">
         <v>60</v>
       </c>
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
@@ -1411,6 +1615,9 @@
       <c r="A62">
         <v>61</v>
       </c>
+      <c r="B62" t="s">
+        <v>15</v>
+      </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
@@ -1428,6 +1635,9 @@
       <c r="A63">
         <v>62</v>
       </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
       <c r="C63" t="s">
         <v>5</v>
       </c>
@@ -1445,6 +1655,9 @@
       <c r="A64">
         <v>63</v>
       </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
@@ -1462,6 +1675,9 @@
       <c r="A65">
         <v>64</v>
       </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
       <c r="C65" t="s">
         <v>3</v>
       </c>
@@ -1479,6 +1695,9 @@
       <c r="A66">
         <v>65</v>
       </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
@@ -1496,6 +1715,9 @@
       <c r="A67">
         <v>66</v>
       </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
       <c r="C67" t="s">
         <v>4</v>
       </c>
@@ -1510,6 +1732,9 @@
       <c r="A68">
         <v>67</v>
       </c>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
       <c r="C68" t="s">
         <v>0</v>
       </c>
@@ -1527,6 +1752,9 @@
       <c r="A69">
         <v>68</v>
       </c>
+      <c r="B69" t="s">
+        <v>16</v>
+      </c>
       <c r="C69" t="s">
         <v>3</v>
       </c>
@@ -1544,6 +1772,9 @@
       <c r="A70">
         <v>69</v>
       </c>
+      <c r="B70" t="s">
+        <v>17</v>
+      </c>
       <c r="C70" t="s">
         <v>0</v>
       </c>
@@ -1561,6 +1792,9 @@
       <c r="A71">
         <v>70</v>
       </c>
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
       <c r="C71" t="s">
         <v>2</v>
       </c>
@@ -1578,6 +1812,9 @@
       <c r="A72">
         <v>71</v>
       </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>
@@ -1595,6 +1832,9 @@
       <c r="A73">
         <v>72</v>
       </c>
+      <c r="B73" t="s">
+        <v>13</v>
+      </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
@@ -1612,6 +1852,9 @@
       <c r="A74">
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>14</v>
+      </c>
       <c r="C74" t="s">
         <v>2</v>
       </c>
@@ -1629,6 +1872,9 @@
       <c r="A75">
         <v>74</v>
       </c>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
       <c r="C75" t="s">
         <v>2</v>
       </c>
@@ -1646,6 +1892,9 @@
       <c r="A76">
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
       <c r="C76" t="s">
         <v>3</v>
       </c>
@@ -1663,6 +1912,9 @@
       <c r="A77">
         <v>76</v>
       </c>
+      <c r="B77" t="s">
+        <v>16</v>
+      </c>
       <c r="C77" t="s">
         <v>6</v>
       </c>
@@ -1680,6 +1932,9 @@
       <c r="A78">
         <v>77</v>
       </c>
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
       <c r="C78" t="s">
         <v>4</v>
       </c>
@@ -1697,6 +1952,9 @@
       <c r="A79">
         <v>78</v>
       </c>
+      <c r="B79" t="s">
+        <v>17</v>
+      </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
@@ -1714,6 +1972,9 @@
       <c r="A80">
         <v>79</v>
       </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
       <c r="C80" t="s">
         <v>0</v>
       </c>
@@ -1731,6 +1992,9 @@
       <c r="A81">
         <v>80</v>
       </c>
+      <c r="B81" t="s">
+        <v>15</v>
+      </c>
       <c r="C81" t="s">
         <v>1</v>
       </c>
@@ -1748,6 +2012,9 @@
       <c r="A82">
         <v>81</v>
       </c>
+      <c r="B82" t="s">
+        <v>14</v>
+      </c>
       <c r="C82" t="s">
         <v>4</v>
       </c>
@@ -1765,6 +2032,9 @@
       <c r="A83">
         <v>82</v>
       </c>
+      <c r="B83" t="s">
+        <v>15</v>
+      </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
@@ -1782,6 +2052,9 @@
       <c r="A84">
         <v>83</v>
       </c>
+      <c r="B84" t="s">
+        <v>16</v>
+      </c>
       <c r="C84" t="s">
         <v>2</v>
       </c>
@@ -1799,6 +2072,9 @@
       <c r="A85">
         <v>84</v>
       </c>
+      <c r="B85" t="s">
+        <v>17</v>
+      </c>
       <c r="C85" t="s">
         <v>0</v>
       </c>
@@ -1816,6 +2092,9 @@
       <c r="A86">
         <v>85</v>
       </c>
+      <c r="B86" t="s">
+        <v>16</v>
+      </c>
       <c r="C86" t="s">
         <v>4</v>
       </c>
@@ -1833,6 +2112,9 @@
       <c r="A87">
         <v>86</v>
       </c>
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
       <c r="C87" t="s">
         <v>2</v>
       </c>
@@ -1850,6 +2132,9 @@
       <c r="A88">
         <v>87</v>
       </c>
+      <c r="B88" t="s">
+        <v>16</v>
+      </c>
       <c r="C88" t="s">
         <v>2</v>
       </c>
@@ -1867,6 +2152,9 @@
       <c r="A89">
         <v>88</v>
       </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
       <c r="C89" t="s">
         <v>0</v>
       </c>
@@ -1884,6 +2172,9 @@
       <c r="A90">
         <v>89</v>
       </c>
+      <c r="B90" t="s">
+        <v>16</v>
+      </c>
       <c r="C90" t="s">
         <v>0</v>
       </c>
@@ -1901,6 +2192,9 @@
       <c r="A91">
         <v>90</v>
       </c>
+      <c r="B91" t="s">
+        <v>15</v>
+      </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
@@ -1918,6 +2212,9 @@
       <c r="A92">
         <v>91</v>
       </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
       <c r="D92" t="s">
         <v>0</v>
       </c>
@@ -1932,6 +2229,9 @@
       <c r="A93">
         <v>92</v>
       </c>
+      <c r="B93" t="s">
+        <v>14</v>
+      </c>
       <c r="C93" t="s">
         <v>3</v>
       </c>
@@ -1949,6 +2249,9 @@
       <c r="A94">
         <v>93</v>
       </c>
+      <c r="B94" t="s">
+        <v>13</v>
+      </c>
       <c r="C94" t="s">
         <v>4</v>
       </c>
@@ -1966,6 +2269,9 @@
       <c r="A95">
         <v>94</v>
       </c>
+      <c r="B95" t="s">
+        <v>16</v>
+      </c>
       <c r="C95" t="s">
         <v>4</v>
       </c>
@@ -1983,6 +2289,9 @@
       <c r="A96">
         <v>95</v>
       </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
       <c r="C96" t="s">
         <v>2</v>
       </c>
@@ -2000,6 +2309,9 @@
       <c r="A97">
         <v>96</v>
       </c>
+      <c r="B97" t="s">
+        <v>17</v>
+      </c>
       <c r="C97" t="s">
         <v>1</v>
       </c>
@@ -2017,6 +2329,9 @@
       <c r="A98">
         <v>97</v>
       </c>
+      <c r="B98" t="s">
+        <v>16</v>
+      </c>
       <c r="C98" t="s">
         <v>5</v>
       </c>
@@ -2034,6 +2349,9 @@
       <c r="A99">
         <v>98</v>
       </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
       <c r="C99" t="s">
         <v>2</v>
       </c>
@@ -2051,6 +2369,9 @@
       <c r="A100">
         <v>99</v>
       </c>
+      <c r="B100" t="s">
+        <v>16</v>
+      </c>
       <c r="C100" t="s">
         <v>3</v>
       </c>
@@ -2068,6 +2389,9 @@
       <c r="A101">
         <v>100</v>
       </c>
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
       <c r="C101" t="s">
         <v>3</v>
       </c>
@@ -2085,6 +2409,9 @@
       <c r="A102">
         <v>101</v>
       </c>
+      <c r="B102" t="s">
+        <v>18</v>
+      </c>
       <c r="C102" t="s">
         <v>0</v>
       </c>
@@ -2102,6 +2429,9 @@
       <c r="A103">
         <v>102</v>
       </c>
+      <c r="B103" t="s">
+        <v>16</v>
+      </c>
       <c r="C103" t="s">
         <v>1</v>
       </c>
@@ -2119,6 +2449,9 @@
       <c r="A104">
         <v>103</v>
       </c>
+      <c r="B104" t="s">
+        <v>13</v>
+      </c>
       <c r="C104" t="s">
         <v>4</v>
       </c>
@@ -2136,6 +2469,9 @@
       <c r="A105">
         <v>104</v>
       </c>
+      <c r="B105" t="s">
+        <v>17</v>
+      </c>
       <c r="D105" t="s">
         <v>0</v>
       </c>
@@ -2150,6 +2486,9 @@
       <c r="A106">
         <v>105</v>
       </c>
+      <c r="B106" t="s">
+        <v>17</v>
+      </c>
       <c r="C106" t="s">
         <v>4</v>
       </c>
@@ -2167,6 +2506,9 @@
       <c r="A107">
         <v>106</v>
       </c>
+      <c r="B107" t="s">
+        <v>18</v>
+      </c>
       <c r="C107" t="s">
         <v>3</v>
       </c>
@@ -2184,6 +2526,9 @@
       <c r="A108">
         <v>107</v>
       </c>
+      <c r="B108" t="s">
+        <v>16</v>
+      </c>
       <c r="C108" t="s">
         <v>3</v>
       </c>
@@ -2201,6 +2546,9 @@
       <c r="A109">
         <v>108</v>
       </c>
+      <c r="B109" t="s">
+        <v>16</v>
+      </c>
       <c r="C109" t="s">
         <v>0</v>
       </c>
@@ -2218,6 +2566,9 @@
       <c r="A110">
         <v>109</v>
       </c>
+      <c r="B110" t="s">
+        <v>14</v>
+      </c>
       <c r="C110" t="s">
         <v>4</v>
       </c>
@@ -2235,6 +2586,9 @@
       <c r="A111">
         <v>110</v>
       </c>
+      <c r="B111" t="s">
+        <v>15</v>
+      </c>
       <c r="C111" t="s">
         <v>2</v>
       </c>
@@ -2252,6 +2606,9 @@
       <c r="A112">
         <v>111</v>
       </c>
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
       <c r="C112" t="s">
         <v>5</v>
       </c>
@@ -2269,6 +2626,9 @@
       <c r="A113">
         <v>112</v>
       </c>
+      <c r="B113" t="s">
+        <v>14</v>
+      </c>
       <c r="C113" t="s">
         <v>1</v>
       </c>
@@ -2286,6 +2646,9 @@
       <c r="A114">
         <v>113</v>
       </c>
+      <c r="B114" t="s">
+        <v>13</v>
+      </c>
       <c r="C114" t="s">
         <v>3</v>
       </c>
@@ -2302,6 +2665,9 @@
     <row r="115" spans="1:6">
       <c r="A115">
         <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>16</v>
       </c>
       <c r="C115" t="s">
         <v>4</v>
@@ -2320,9 +2686,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2549,27 +2918,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F81E27C1-977A-425C-AA82-8308CB8EABF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A9E69D-4B7A-4D74-86BF-701F80200025}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="5bb98f44-fee0-4296-b2c2-b5adab6c8af1"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0559e13a-8544-42a8-90f8-5f2be42cf9d1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2594,9 +2951,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81A9E69D-4B7A-4D74-86BF-701F80200025}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F81E27C1-977A-425C-AA82-8308CB8EABF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="5bb98f44-fee0-4296-b2c2-b5adab6c8af1"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0559e13a-8544-42a8-90f8-5f2be42cf9d1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>